<commit_message>
Design Drawing Form commit
</commit_message>
<xml_diff>
--- a/wcrfrontend/public/files/designDrawing/Designs_Drawings.xlsx
+++ b/wcrfrontend/public/files/designDrawing/Designs_Drawings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vikas\git\wcrpmis\wcrfrontend\public\files\designDrawing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14C3005-2D51-4CF4-B07B-DBB9AEC0E317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD79B61-D6C2-46BE-A7FC-F6C9B8E86ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Design &amp; Drawing" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
-  <si>
-    <t>Unique ID of the Work</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>Department to which the design or drawing belongs to</t>
   </si>
@@ -38,18 +35,9 @@
     <t>Drawing prepared By from reference table</t>
   </si>
   <si>
-    <t>Contract ID of the consultant preparing the drawing (If prepared by MRVC or Contractor, leave blank)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Proof Consultant Contract ID checking the design/ drg.(Leave blank if no proof checking) </t>
   </si>
   <si>
-    <t>Type of Drawing</t>
-  </si>
-  <si>
-    <t>Title of the drawing</t>
-  </si>
-  <si>
     <t>Drawing No assigned by the Agency</t>
   </si>
   <si>
@@ -65,9 +53,6 @@
     <t>Any additional remarks</t>
   </si>
   <si>
-    <t>PMIS Drawing No</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Contract ID</t>
   </si>
   <si>
@@ -158,10 +143,16 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>Upload File</t>
-  </si>
-  <si>
-    <t>Current (Y/N)</t>
+    <t>Design Sequence Id</t>
+  </si>
+  <si>
+    <t>Unique ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Required </t>
+  </si>
+  <si>
+    <t>Required</t>
   </si>
 </sst>
 </file>
@@ -575,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -584,155 +575,149 @@
     <col min="1" max="25" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="46" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -742,41 +727,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I5"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="35" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>